<commit_message>
Correction de doc en grande partie
</commit_message>
<xml_diff>
--- a/Documentation/documents/Planning_TPI_Jauch.xlsx
+++ b/Documentation/documents/Planning_TPI_Jauch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wal41\source\repos\LogoGo\Documentation\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BACBD08E-D3FA-42AF-8093-A63C59A9C837}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EAD3B78-37B1-41F0-B886-26A33DAB8DE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5112" yWindow="348" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionel" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="98">
   <si>
     <t>Jour</t>
   </si>
@@ -341,13 +341,16 @@
     <t>Total 8.juin</t>
   </si>
   <si>
-    <t>Doc toute la journée</t>
-  </si>
-  <si>
     <t>Doxygen, Latex</t>
   </si>
   <si>
     <t>Uniquement de la doc…Reste pas grand-chose</t>
+  </si>
+  <si>
+    <t>Doc toute la journée --&gt; génération Doxygen + LaTex après recommendations de M. Bonvin</t>
+  </si>
+  <si>
+    <t>Rien à ajouter. Bonne journée.</t>
   </si>
 </sst>
 </file>
@@ -682,7 +685,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -848,6 +851,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1681,8 +1687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:X16"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="V14" sqref="V14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA14" sqref="AA14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2052,7 +2058,7 @@
       <c r="T12" s="46"/>
       <c r="U12" s="46"/>
       <c r="V12" s="46"/>
-      <c r="W12" s="40"/>
+      <c r="W12" s="46"/>
       <c r="X12" s="41"/>
     </row>
     <row r="13" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2106,8 +2112,8 @@
       <c r="T14" s="40"/>
       <c r="U14" s="40"/>
       <c r="V14" s="40"/>
-      <c r="W14" s="40"/>
-      <c r="X14" s="41"/>
+      <c r="W14" s="46"/>
+      <c r="X14" s="56"/>
     </row>
     <row r="15" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="15" t="s">
@@ -2160,8 +2166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="G58" sqref="G58"/>
+    <sheetView topLeftCell="A49" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="36.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2903,6 +2909,9 @@
         <f>SUM(C53:C54)</f>
         <v>0.33333333333333331</v>
       </c>
+      <c r="D55" s="9" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="56" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="6">
@@ -2915,7 +2924,7 @@
         <v>0.27083333333333331</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2929,7 +2938,7 @@
         <v>6.25E-2</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="58" spans="1:4" s="9" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2943,8 +2952,8 @@
         <f>SUM(C56:C57)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D58" s="2" t="s">
-        <v>96</v>
+      <c r="D58" s="9" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ajout du zip contenant la doc générée par doxygen
</commit_message>
<xml_diff>
--- a/Documentation/documents/Planning_TPI_Jauch.xlsx
+++ b/Documentation/documents/Planning_TPI_Jauch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wal41\source\repos\LogoGo\Documentation\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EAD3B78-37B1-41F0-B886-26A33DAB8DE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F6E488-C35A-48F1-BAD0-A73BFF7C638B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="102">
   <si>
     <t>Jour</t>
   </si>
@@ -351,6 +351,18 @@
   </si>
   <si>
     <t>Rien à ajouter. Bonne journée.</t>
+  </si>
+  <si>
+    <t>Total 9.juin</t>
+  </si>
+  <si>
+    <t>Finalisations</t>
+  </si>
+  <si>
+    <t>Relecture de doc et de code. Correction d'images, etc.</t>
+  </si>
+  <si>
+    <t>Fini.</t>
   </si>
 </sst>
 </file>
@@ -894,8 +906,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:D58" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D58" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:D61" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D61" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tâche" dataDxfId="2"/>
@@ -2164,10 +2176,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K64"/>
+  <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView topLeftCell="A53" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="36.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2957,35 +2969,64 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="9"/>
-      <c r="B59" s="9"/>
-      <c r="C59" s="10"/>
+      <c r="A59" s="6">
+        <v>43991</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C59" s="7">
+        <v>0.3125</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="60" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="9"/>
-      <c r="B60" s="9"/>
-      <c r="C60" s="10"/>
-      <c r="D60" s="9"/>
+      <c r="A60" s="6">
+        <v>43991</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C60" s="7">
+        <v>2.0833333333333332E-2</v>
+      </c>
     </row>
     <row r="61" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="6"/>
-      <c r="C61" s="3"/>
+      <c r="A61" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C61" s="10">
+        <f>SUM(C59:C60)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="62" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="6"/>
       <c r="C62" s="3"/>
     </row>
-    <row r="63" spans="1:4" s="9" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="6"/>
-      <c r="B63" s="2"/>
       <c r="C63" s="3"/>
-      <c r="D63" s="2"/>
-    </row>
-    <row r="64" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="9"/>
-      <c r="B64" s="10"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="9"/>
+    </row>
+    <row r="64" spans="1:4" s="9" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="6"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="2"/>
+    </row>
+    <row r="65" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="9"/>
+      <c r="B65" s="10"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>